<commit_message>
add the data for different depth
</commit_message>
<xml_diff>
--- a/ILP/NN/hyperpara.xlsx
+++ b/ILP/NN/hyperpara.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131CE50-BDF3-43AF-83DC-BB96853D727B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D821C0-B530-426A-8FFD-C04886D88F31}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3500" yWindow="5920" windowWidth="10200" windowHeight="5010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1e3" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="3e3" sheetId="3" r:id="rId3"/>
     <sheet name="4e3" sheetId="4" r:id="rId4"/>
     <sheet name="5e3" sheetId="5" r:id="rId5"/>
+    <sheet name="Addition" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="93">
   <si>
     <t>hidden layer</t>
   </si>
@@ -303,6 +304,18 @@
   <si>
     <t>training dataset size=5000, batchsize=1000, epochs=40, learning rate=0.001</t>
   </si>
+  <si>
+    <t>training dataset size=1024, batchsize=64, learning rate=0.001</t>
+  </si>
+  <si>
+    <t>epochs\layers</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
 </sst>
 </file>
 
@@ -360,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -705,7 +721,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,43 +735,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="7">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="7">
         <v>5</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="7">
         <v>2</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="7">
         <v>1</v>
       </c>
@@ -1329,34 +1345,34 @@
       <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1917,34 +1933,34 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="S23" s="6" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
@@ -2505,34 +2521,34 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="M34" s="6" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="M34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="S34" s="6" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="S34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -3164,22 +3180,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="S12:W12"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="S34:W34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="S34:W34"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="S12:W12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3204,43 +3220,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="7">
         <v>20</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="7">
         <v>10</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="7">
         <v>4</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="7">
         <v>2</v>
       </c>
@@ -3816,34 +3832,34 @@
       <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -4404,34 +4420,34 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="S23" s="6" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -4992,34 +5008,34 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="M34" s="6" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="M34" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="S34" s="6" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="S34" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -5651,6 +5667,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="S34:W34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
@@ -5659,14 +5683,6 @@
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="M12:Q12"/>
     <mergeCell ref="S12:W12"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="S34:W34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5691,43 +5707,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="7">
         <v>30</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="7">
         <v>15</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="7">
         <v>6</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="7">
         <v>3</v>
       </c>
@@ -6303,34 +6319,34 @@
       <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -6891,34 +6907,34 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="S23" s="6" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -7479,34 +7495,34 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="M34" s="6" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="M34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="S34" s="6" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="S34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -8138,6 +8154,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="S34:W34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
@@ -8146,14 +8170,6 @@
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="M12:Q12"/>
     <mergeCell ref="S12:W12"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="S34:W34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8165,7 +8181,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L6" sqref="H5:L6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8178,43 +8194,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="7">
         <v>40</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="7">
         <v>20</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="7">
         <v>8</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="7">
         <v>4</v>
       </c>
@@ -8790,34 +8806,34 @@
       <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -9378,34 +9394,34 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="S23" s="6" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -9966,34 +9982,34 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="M34" s="6" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="M34" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="S34" s="6" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="S34" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -10625,6 +10641,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="S34:W34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
@@ -10633,14 +10657,6 @@
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="M12:Q12"/>
     <mergeCell ref="S12:W12"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="S34:W34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -10651,8 +10667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBEB8D8-7776-40C9-B813-21A4A04E81D5}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W42" sqref="W42"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10665,43 +10681,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="7">
         <v>50</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="7">
         <v>25</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="7">
         <v>10</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="7">
         <v>5</v>
       </c>
@@ -11279,34 +11295,34 @@
       <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -11867,34 +11883,34 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="S23" s="6" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -12455,34 +12471,34 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="M34" s="6" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="M34" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="S34" s="6" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="S34" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -13114,6 +13130,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="S34:W34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
@@ -13122,14 +13146,514 @@
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="M12:Q12"/>
     <mergeCell ref="S12:W12"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="S34:W34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23508D09-EE3B-4A03-87CB-C11F993E9737}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.64690000000000003</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.60450000000000004</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.38279999999999997</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.82030000000000003</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.85309999999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.85470000000000002</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.75939999999999996</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.70779999999999998</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.85309999999999997</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.82809999999999995</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.9234</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.88280000000000003</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.95940000000000003</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.92190000000000005</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.98129999999999995</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.97340000000000004</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.94379999999999997</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.92190000000000005</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.94530000000000003</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.97030000000000005</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.96409999999999996</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.96409999999999996</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.98129999999999995</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.93589999999999995</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.95940000000000003</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.746</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.745</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.748</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.749</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.752</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="G24" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>